<commit_message>
Various fixes for testing resource requests
</commit_message>
<xml_diff>
--- a/resources/data-imports/Kingdoms/kingdoms.xlsx
+++ b/resources/data-imports/Kingdoms/kingdoms.xlsx
@@ -717,7 +717,7 @@
     <col min="30" max="30" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="31" max="31" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="32" max="32" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="33" max="33" width="29.421" bestFit="true" customWidth="true" style="0"/>
     <col min="34" max="34" width="17.567" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -1650,8 +1650,8 @@
       <c r="AE12">
         <v>1</v>
       </c>
-      <c r="AG12">
-        <v>5</v>
+      <c r="AG12" t="s">
+        <v>54</v>
       </c>
       <c r="AH12">
         <v>1</v>
@@ -1739,8 +1739,8 @@
       <c r="AE13">
         <v>1</v>
       </c>
-      <c r="AG13">
-        <v>7</v>
+      <c r="AG13" t="s">
+        <v>56</v>
       </c>
       <c r="AH13">
         <v>1</v>
@@ -1825,8 +1825,8 @@
       <c r="AE14">
         <v>1</v>
       </c>
-      <c r="AG14">
-        <v>9</v>
+      <c r="AG14" t="s">
+        <v>58</v>
       </c>
       <c r="AH14">
         <v>1</v>
@@ -1908,8 +1908,8 @@
       <c r="AF15">
         <v>1</v>
       </c>
-      <c r="AG15">
-        <v>10</v>
+      <c r="AG15" t="s">
+        <v>60</v>
       </c>
       <c r="AH15">
         <v>1</v>
@@ -1997,8 +1997,8 @@
       <c r="AF16">
         <v>1</v>
       </c>
-      <c r="AG16">
-        <v>12</v>
+      <c r="AG16" t="s">
+        <v>62</v>
       </c>
       <c r="AH16">
         <v>1</v>
@@ -2075,6 +2075,12 @@
         <v>15</v>
       </c>
       <c r="AE17">
+        <v>1</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH17">
         <v>1</v>
       </c>
     </row>

</xml_diff>